<commit_message>
Changed Code as per latest Deployment and fixed Biannual Cases too
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/ExportExcel.xlsx
+++ b/src/main/resources/TestData/ExportExcel.xlsx
@@ -890,8 +890,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="72.6275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.8724489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1328,17 +1327,16 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3520408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.98469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added script to run leaves omnly for four edge days
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/ExportExcel.xlsx
+++ b/src/main/resources/TestData/ExportExcel.xlsx
@@ -1504,8 +1504,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.0969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.7448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1942,17 +1942,18 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.4081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.7908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1999,8 +2000,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2035,12 +2035,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Changed scenarios to run on jenkins
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/ExportExcel.xlsx
+++ b/src/main/resources/TestData/ExportExcel.xlsx
@@ -1504,8 +1504,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.7448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.9387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1942,18 +1942,18 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.7908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="68.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2000,7 +2000,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2035,12 +2036,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0714285714286"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>